<commit_message>
finding chi2/ndof=1 for some data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronlv\PycharmProjects\LabScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8261F-30CB-4D78-8064-11B50B2401EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29A6ECB-90FA-4A8A-9210-374435F6B091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA83AA4A-F2AA-4645-AE70-6E9620D9E046}"/>
+    <workbookView xWindow="5388" yWindow="5004" windowWidth="17280" windowHeight="8964" xr2:uid="{FA83AA4A-F2AA-4645-AE70-6E9620D9E046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AF9FDB-A199-437A-9646-D42047FCB923}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,10 +422,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>0.01</v>
@@ -436,10 +436,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>0.01</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.11</v>
+        <v>0.16</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C4">
         <v>0.01</v>
@@ -464,10 +464,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="B5">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>0.01</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.21</v>
+        <v>0.26</v>
       </c>
       <c r="B6">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C6">
         <v>0.01</v>
@@ -492,29 +492,15 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
       <c r="B7">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="C7">
         <v>0.01</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0.31</v>
-      </c>
-      <c r="B8">
-        <v>180</v>
-      </c>
-      <c r="C8">
-        <v>0.01</v>
-      </c>
-      <c r="D8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added simple plot option
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronlv\PycharmProjects\LabScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B652DAB9-0941-44EC-BF92-FA2FCFB70D48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD947519-BD8D-402C-A25F-73577034F294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5655" yWindow="1455" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -378,13 +378,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>-0.77700000000000002</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>450</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -392,75 +392,104 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>-0.55100000000000005</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>500</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>-0.52900000000000003</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>503</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>-0.42699999999999999</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>525</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>-0.35199999999999998</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>540</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>552</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-0.26200000000000001</v>
+      </c>
+      <c r="B8">
+        <v>575</v>
+      </c>
+      <c r="C8">
+        <v>1E-3</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>-0.17269999999999999</v>
+      </c>
+      <c r="B9">
+        <v>602</v>
+      </c>
+      <c r="C9">
+        <v>1E-4</v>
+      </c>
+      <c r="D9">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>